<commit_message>
path and code correction
</commit_message>
<xml_diff>
--- a/Data_Transformer/Logs Remove Duplicate for Dashboard.xlsx
+++ b/Data_Transformer/Logs Remove Duplicate for Dashboard.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
@@ -734,6 +734,100 @@
         <v>393</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Akash Shahapure</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4.836565017700195</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>03/07/2024 16:55:38</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>03/07/2024 16:58:56</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>198</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>cases_report_Tata Power (Maithon Power Ltd)_(All States)_2024-06-19</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>17916</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Akash Shahapure</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.836565017700195</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>03/07/2024 16:55:38</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>03/07/2024 16:59:06</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>208</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>cases_report_Tata Power (Maithon Power Ltd)_(All States)_2024-06-19</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>17917</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>393</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
st.experimental_rerun() depricated hence changed to st.rerun()
</commit_message>
<xml_diff>
--- a/Data_Transformer/Logs Remove Duplicate for Dashboard.xlsx
+++ b/Data_Transformer/Logs Remove Duplicate for Dashboard.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
@@ -828,6 +828,476 @@
         <v>393</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:23:55</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:24:35</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>40</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J9" t="n">
+        <v>4</v>
+      </c>
+      <c r="K9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:23:55</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:24:37</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>43</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>2921</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4</v>
+      </c>
+      <c r="K10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:23:55</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:24:47</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>52</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4</v>
+      </c>
+      <c r="K11" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:23:55</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:24:51</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>56</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:23:55</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>16/07/2024 16:24:53</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>59</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>2921</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4</v>
+      </c>
+      <c r="K13" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:03</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:45</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>43</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4</v>
+      </c>
+      <c r="K14" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:03</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:48</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>45</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>2921</v>
+      </c>
+      <c r="J15" t="n">
+        <v>4</v>
+      </c>
+      <c r="K15" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:03</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:12:58</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>115</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:03</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:13:01</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>118</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4</v>
+      </c>
+      <c r="K17" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Akash Shahapure Test</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>akash.shahapure@haqdarshak.com</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.7465200424194336</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:11:03</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>16/07/2024 18:13:05</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>122</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>cases_report_Shapoorji Pallonji Group_MH_(All States)_2024-07-16</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>2921</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4</v>
+      </c>
+      <c r="K18" t="n">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>